<commit_message>
Optimised use of pandas and added colours!
</commit_message>
<xml_diff>
--- a/test_spreadsheet.xlsx
+++ b/test_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\vorn-finance-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E1B022-8B20-4346-BEAB-64B7ABB4BCF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EFFC53-0BEE-4C36-A291-B1D7D99A595C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -701,8 +701,8 @@
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
     <col min="2" max="15" width="14.42578125" style="11" customWidth="1"/>
     <col min="16" max="16" width="23.140625" style="11" customWidth="1"/>
-    <col min="17" max="34" width="14.42578125" style="11" customWidth="1"/>
-    <col min="35" max="16384" width="14.42578125" style="11"/>
+    <col min="17" max="36" width="14.42578125" style="11" customWidth="1"/>
+    <col min="37" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ability to ignore transactions and fixed some bugs.
</commit_message>
<xml_diff>
--- a/test_spreadsheet.xlsx
+++ b/test_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\vorn-finance-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EFFC53-0BEE-4C36-A291-B1D7D99A595C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63EB63-64DF-40D3-B5F7-D2F72D2165F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -701,8 +701,8 @@
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
     <col min="2" max="15" width="14.42578125" style="11" customWidth="1"/>
     <col min="16" max="16" width="23.140625" style="11" customWidth="1"/>
-    <col min="17" max="36" width="14.42578125" style="11" customWidth="1"/>
-    <col min="37" max="16384" width="14.42578125" style="11"/>
+    <col min="17" max="37" width="14.42578125" style="11" customWidth="1"/>
+    <col min="38" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved user experience and added support for more CSV structures
</commit_message>
<xml_diff>
--- a/test_spreadsheet.xlsx
+++ b/test_spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\vorn-finance-tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Projects\vorn-finance-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63EB63-64DF-40D3-B5F7-D2F72D2165F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A881132-FC0A-40B7-89BA-58A5F7460D73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -701,8 +701,8 @@
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
     <col min="2" max="15" width="14.42578125" style="11" customWidth="1"/>
     <col min="16" max="16" width="23.140625" style="11" customWidth="1"/>
-    <col min="17" max="37" width="14.42578125" style="11" customWidth="1"/>
-    <col min="38" max="16384" width="14.42578125" style="11"/>
+    <col min="17" max="38" width="14.42578125" style="11" customWidth="1"/>
+    <col min="39" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>